<commit_message>
added cash models, added view handler for payment_AR
</commit_message>
<xml_diff>
--- a/aCCTg. pROGRAm/PAYMENT A-R.xlsx
+++ b/aCCTg. pROGRAm/PAYMENT A-R.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,6 +122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -426,9 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="A1:G9"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -479,10 +478,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,16 +489,17 @@
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D3" s="3">
         <v>5000</v>
       </c>
@@ -522,7 +522,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -533,12 +533,13 @@
         <f>+F3-E4</f>
         <v>4000</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -551,7 +552,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -564,7 +565,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -572,7 +573,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -581,14 +582,14 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>0</v>
       </c>
@@ -599,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>18000</v>
       </c>

</xml_diff>

<commit_message>
added generate buyer transactions
</commit_message>
<xml_diff>
--- a/aCCTg. pROGRAm/PAYMENT A-R.xlsx
+++ b/aCCTg. pROGRAm/PAYMENT A-R.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>DR</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>CASH ON HAND LEDGER</t>
+  </si>
+  <si>
+    <t>get date</t>
+  </si>
+  <si>
+    <t>get amount</t>
+  </si>
+  <si>
+    <t>set balance</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>pa</t>
   </si>
 </sst>
 </file>
@@ -116,13 +131,13 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -438,16 +453,16 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -478,10 +493,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,14 +507,14 @@
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
@@ -510,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" s="3">
         <v>5000</v>
       </c>
@@ -521,8 +536,14 @@
         <f>+D3</f>
         <v>5000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -533,13 +554,27 @@
         <f>+F3-E4</f>
         <v>4000</v>
       </c>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -551,8 +586,14 @@
         <f>+F4+D6</f>
         <v>7000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -564,8 +605,26 @@
         <f>+F6-E7</f>
         <v>5000</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <f>+K5-K7</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -573,7 +632,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -582,14 +641,14 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="7" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>0</v>
       </c>
@@ -600,7 +659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>18000</v>
       </c>

</xml_diff>